<commit_message>
added linebreak in excel sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/files/AyurBaby.xlsx
+++ b/src/main/resources/files/AyurBaby.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="25600" windowHeight="15620" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="35100" yWindow="860" windowWidth="25600" windowHeight="15620" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="nutritional" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="175">
   <si>
     <t>Month</t>
   </si>
@@ -279,12 +279,6 @@
   </si>
   <si>
     <t>Which foods are a good source of iron?</t>
-  </si>
-  <si>
-    <t>Vegetables: Brewed black tea, Kale (seaweed), spinach.</t>
-  </si>
-  <si>
-    <t>Pulses, cereals &amp; nuts: Black beans, whole oatmeal, whole wheat pasta, brown rice, nuts.</t>
   </si>
   <si>
     <t>Zinc</t>
@@ -558,7 +552,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -608,6 +602,10 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -1134,15 +1132,15 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="13">
       <c r="A2" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -1151,12 +1149,12 @@
         <v>11</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="26">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>8</v>
@@ -1176,13 +1174,13 @@
     </row>
     <row r="4" spans="1:9" ht="13">
       <c r="A4" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>11</v>
@@ -1190,28 +1188,28 @@
     </row>
     <row r="5" spans="1:9" ht="13">
       <c r="A5" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" ht="39">
       <c r="A6" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>13</v>
@@ -1219,10 +1217,10 @@
     </row>
     <row r="7" spans="1:9" ht="13">
       <c r="A7" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
@@ -1232,10 +1230,10 @@
     </row>
     <row r="8" spans="1:9" ht="13">
       <c r="A8" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
@@ -1245,7 +1243,7 @@
     </row>
     <row r="9" spans="1:9" ht="13">
       <c r="A9" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>16</v>
@@ -1256,18 +1254,18 @@
     </row>
     <row r="10" spans="1:9" ht="13">
       <c r="A10" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>19</v>
@@ -1284,10 +1282,10 @@
     </row>
     <row r="12" spans="1:9" ht="13">
       <c r="A12" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>15</v>
@@ -1295,7 +1293,7 @@
     </row>
     <row r="13" spans="1:9" ht="13">
       <c r="A13" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>22</v>
@@ -1309,7 +1307,7 @@
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>25</v>
@@ -1323,7 +1321,7 @@
     </row>
     <row r="15" spans="1:9" ht="13">
       <c r="A15" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>27</v>
@@ -1334,7 +1332,7 @@
     </row>
     <row r="16" spans="1:9" ht="26">
       <c r="A16" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>29</v>
@@ -1348,7 +1346,7 @@
     </row>
     <row r="17" spans="1:6" ht="13">
       <c r="A17" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>32</v>
@@ -1359,10 +1357,10 @@
     </row>
     <row r="18" spans="1:6" ht="13">
       <c r="A18" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>33</v>
@@ -1373,7 +1371,7 @@
     </row>
     <row r="19" spans="1:6" ht="13">
       <c r="A19" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>29</v>
@@ -1384,10 +1382,10 @@
     </row>
     <row r="20" spans="1:6" ht="13">
       <c r="A20" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>36</v>
@@ -1395,7 +1393,7 @@
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>37</v>
@@ -1406,7 +1404,7 @@
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>39</v>
@@ -1420,18 +1418,18 @@
     </row>
     <row r="23" spans="1:6" ht="13">
       <c r="A23" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="26">
       <c r="A24" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>42</v>
@@ -1439,7 +1437,7 @@
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>44</v>
@@ -1447,19 +1445,19 @@
     </row>
     <row r="26" spans="1:6" ht="13">
       <c r="A26" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>46</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>47</v>
@@ -1467,13 +1465,13 @@
     </row>
     <row r="27" spans="1:6" ht="26">
       <c r="A27" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>46</v>
@@ -1484,21 +1482,21 @@
     </row>
     <row r="28" spans="1:6" ht="13">
       <c r="A28" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="13">
       <c r="A29" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>54</v>
@@ -1507,7 +1505,7 @@
         <v>55</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1523,10 +1521,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A137"/>
+  <dimension ref="A1:A132"/>
   <sheetViews>
-    <sheetView topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1541,12 +1539,12 @@
     </row>
     <row r="2" spans="1:1" ht="15" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15" customHeight="1">
       <c r="A3" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15" customHeight="1">
@@ -1589,7 +1587,7 @@
     </row>
     <row r="12" spans="1:1" ht="15" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15" customHeight="1">
@@ -1602,7 +1600,7 @@
     </row>
     <row r="15" spans="1:1" ht="15" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15" customHeight="1">
@@ -1643,7 +1641,7 @@
     </row>
     <row r="24" spans="1:1" ht="15" customHeight="1">
       <c r="A24" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15" customHeight="1">
@@ -1758,382 +1756,360 @@
         <v>84</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="15" customHeight="1">
-      <c r="A50" s="1"/>
-    </row>
     <row r="51" spans="1:1" ht="15" customHeight="1">
       <c r="A51" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="15" customHeight="1">
-      <c r="A52" s="7" t="s">
-        <v>77</v>
+      <c r="A52" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="15" customHeight="1">
       <c r="A53" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="15" customHeight="1">
-      <c r="A54" s="7" t="s">
-        <v>87</v>
+      <c r="A54" s="1"/>
+    </row>
+    <row r="55" spans="1:1" ht="15" customHeight="1">
+      <c r="A55" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="15" customHeight="1">
-      <c r="A56" s="1" t="s">
-        <v>88</v>
+      <c r="A56" s="7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="15" customHeight="1">
-      <c r="A57" s="1" t="s">
-        <v>89</v>
-      </c>
+      <c r="A57" s="1"/>
     </row>
     <row r="58" spans="1:1" ht="15" customHeight="1">
-      <c r="A58" s="7" t="s">
+      <c r="A58" s="1" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="15" customHeight="1">
-      <c r="A59" s="1"/>
+      <c r="A59" s="7" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="60" spans="1:1" ht="15" customHeight="1">
-      <c r="A60" s="1" t="s">
-        <v>62</v>
+      <c r="A60" s="7" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="15" customHeight="1">
       <c r="A61" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" ht="15" customHeight="1">
-      <c r="A62" s="1"/>
+        <v>93</v>
+      </c>
     </row>
     <row r="63" spans="1:1" ht="15" customHeight="1">
       <c r="A63" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="15" customHeight="1">
-      <c r="A64" s="7" t="s">
-        <v>93</v>
+      <c r="A64" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="15" customHeight="1">
       <c r="A65" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="15" customHeight="1">
-      <c r="A66" s="7" t="s">
-        <v>95</v>
+      <c r="A66" s="1"/>
+    </row>
+    <row r="67" spans="1:1" ht="15" customHeight="1">
+      <c r="A67" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="15" customHeight="1">
-      <c r="A68" s="1" t="s">
-        <v>96</v>
+      <c r="A68" s="7" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="15" customHeight="1">
-      <c r="A69" s="1" t="s">
-        <v>97</v>
-      </c>
+      <c r="A69" s="1"/>
     </row>
     <row r="70" spans="1:1" ht="15" customHeight="1">
-      <c r="A70" s="7" t="s">
+      <c r="A70" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="15" customHeight="1">
+      <c r="A71" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="15" customHeight="1">
-      <c r="A71" s="1"/>
-    </row>
     <row r="72" spans="1:1" ht="15" customHeight="1">
-      <c r="A72" s="1" t="s">
-        <v>62</v>
+      <c r="A72" s="7" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="15" customHeight="1">
       <c r="A73" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="15" customHeight="1">
-      <c r="A74" s="1"/>
-    </row>
-    <row r="75" spans="1:1" ht="15" customHeight="1">
-      <c r="A75" s="1" t="s">
+      <c r="A74" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="15" customHeight="1">
+      <c r="A76" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="15" customHeight="1">
+      <c r="A77" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" ht="15" customHeight="1">
+      <c r="A78" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" ht="15" customHeight="1">
+      <c r="A79" s="2"/>
+    </row>
+    <row r="80" spans="1:1" ht="15" customHeight="1">
+      <c r="A80" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="15" customHeight="1">
+      <c r="A81" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" ht="15" customHeight="1">
+      <c r="A82" s="1"/>
+    </row>
+    <row r="83" spans="1:1" ht="15" customHeight="1">
+      <c r="A83" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="15" customHeight="1">
-      <c r="A76" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" ht="15" customHeight="1">
-      <c r="A77" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" ht="15" customHeight="1">
-      <c r="A78" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" ht="15" customHeight="1">
-      <c r="A79" s="7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" ht="15" customHeight="1">
-      <c r="A81" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" ht="15" customHeight="1">
-      <c r="A82" s="1" t="s">
+    <row r="84" spans="1:1" ht="15" customHeight="1">
+      <c r="A84" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="15" customHeight="1">
-      <c r="A83" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" ht="15" customHeight="1">
-      <c r="A84" s="2"/>
-    </row>
     <row r="85" spans="1:1" ht="15" customHeight="1">
-      <c r="A85" s="1" t="s">
-        <v>62</v>
+      <c r="A85" s="7" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="15" customHeight="1">
       <c r="A86" s="7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" ht="15" customHeight="1">
-      <c r="A87" s="1"/>
+        <v>107</v>
+      </c>
     </row>
     <row r="88" spans="1:1" ht="15" customHeight="1">
       <c r="A88" s="1" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="15" customHeight="1">
-      <c r="A89" s="7" t="s">
-        <v>107</v>
+      <c r="A89" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="15" customHeight="1">
       <c r="A90" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="91" spans="1:1" ht="15" customHeight="1">
-      <c r="A91" s="7" t="s">
-        <v>109</v>
+      <c r="A91" s="1"/>
+    </row>
+    <row r="92" spans="1:1" ht="15" customHeight="1">
+      <c r="A92" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="15" customHeight="1">
-      <c r="A93" s="1" t="s">
-        <v>110</v>
+      <c r="A93" s="7" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="15" customHeight="1">
-      <c r="A94" s="1" t="s">
-        <v>111</v>
-      </c>
+      <c r="A94" s="1"/>
     </row>
     <row r="95" spans="1:1" ht="15" customHeight="1">
-      <c r="A95" s="7" t="s">
+      <c r="A95" s="1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="15" customHeight="1">
-      <c r="A96" s="1"/>
+      <c r="A96" s="7" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="97" spans="1:1" ht="15" customHeight="1">
-      <c r="A97" s="1" t="s">
-        <v>62</v>
+      <c r="A97" s="7" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="98" spans="1:1" ht="15" customHeight="1">
       <c r="A98" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="99" spans="1:1" ht="15" customHeight="1">
-      <c r="A99" s="1"/>
-    </row>
-    <row r="100" spans="1:1" ht="15" customHeight="1">
-      <c r="A100" s="1" t="s">
-        <v>114</v>
+      <c r="A99" s="7" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="101" spans="1:1" ht="15" customHeight="1">
-      <c r="A101" s="7" t="s">
-        <v>115</v>
+      <c r="A101" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="102" spans="1:1" ht="15" customHeight="1">
-      <c r="A102" s="7" t="s">
-        <v>116</v>
+      <c r="A102" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="103" spans="1:1" ht="15" customHeight="1">
       <c r="A103" s="7" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="104" spans="1:1" ht="15" customHeight="1">
-      <c r="A104" s="7" t="s">
-        <v>118</v>
+      <c r="A104" s="1"/>
+    </row>
+    <row r="105" spans="1:1" ht="15" customHeight="1">
+      <c r="A105" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="106" spans="1:1" ht="15" customHeight="1">
-      <c r="A106" s="1" t="s">
-        <v>119</v>
+      <c r="A106" s="7" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="107" spans="1:1" ht="15" customHeight="1">
-      <c r="A107" s="1" t="s">
-        <v>120</v>
-      </c>
+      <c r="A107" s="1"/>
     </row>
     <row r="108" spans="1:1" ht="15" customHeight="1">
-      <c r="A108" s="7" t="s">
+      <c r="A108" s="1" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="109" spans="1:1" ht="15" customHeight="1">
-      <c r="A109" s="1"/>
+      <c r="A109" s="7" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="110" spans="1:1" ht="15" customHeight="1">
-      <c r="A110" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" ht="15" customHeight="1">
-      <c r="A111" s="7" t="s">
-        <v>122</v>
+      <c r="A110" s="7" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="15" customHeight="1">
-      <c r="A112" s="1"/>
+      <c r="A112" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="113" spans="1:1" ht="15" customHeight="1">
       <c r="A113" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="114" spans="1:1" ht="15" customHeight="1">
       <c r="A114" s="7" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="115" spans="1:1" ht="15" customHeight="1">
-      <c r="A115" s="7" t="s">
-        <v>125</v>
+      <c r="A115" s="1"/>
+    </row>
+    <row r="116" spans="1:1" ht="15" customHeight="1">
+      <c r="A116" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="117" spans="1:1" ht="15" customHeight="1">
-      <c r="A117" s="1" t="s">
-        <v>126</v>
+      <c r="A117" s="7" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="118" spans="1:1" ht="15" customHeight="1">
-      <c r="A118" s="1" t="s">
-        <v>127</v>
-      </c>
+      <c r="A118" s="1"/>
     </row>
     <row r="119" spans="1:1" ht="15" customHeight="1">
-      <c r="A119" s="7" t="s">
+      <c r="A119" s="1" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="120" spans="1:1" ht="15" customHeight="1">
-      <c r="A120" s="1"/>
+      <c r="A120" s="7" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="121" spans="1:1" ht="15" customHeight="1">
-      <c r="A121" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" ht="15" customHeight="1">
-      <c r="A122" s="7" t="s">
-        <v>129</v>
+      <c r="A121" s="7" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="123" spans="1:1" ht="15" customHeight="1">
-      <c r="A123" s="1"/>
+      <c r="A123" s="1" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="124" spans="1:1" ht="15" customHeight="1">
       <c r="A124" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="125" spans="1:1" ht="15" customHeight="1">
       <c r="A125" s="7" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="126" spans="1:1" ht="15" customHeight="1">
-      <c r="A126" s="7" t="s">
-        <v>132</v>
+      <c r="A126" s="1"/>
+    </row>
+    <row r="127" spans="1:1" ht="15" customHeight="1">
+      <c r="A127" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="128" spans="1:1" ht="15" customHeight="1">
-      <c r="A128" s="1" t="s">
-        <v>133</v>
+      <c r="A128" s="7" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="129" spans="1:1" ht="15" customHeight="1">
-      <c r="A129" s="1" t="s">
-        <v>134</v>
-      </c>
+      <c r="A129" s="1"/>
     </row>
     <row r="130" spans="1:1" ht="15" customHeight="1">
-      <c r="A130" s="7" t="s">
+      <c r="A130" s="1" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="131" spans="1:1" ht="15" customHeight="1">
-      <c r="A131" s="1"/>
+      <c r="A131" s="7" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="132" spans="1:1" ht="15" customHeight="1">
-      <c r="A132" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" ht="15" customHeight="1">
-      <c r="A133" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" ht="15" customHeight="1">
-      <c r="A134" s="1"/>
-    </row>
-    <row r="135" spans="1:1" ht="15" customHeight="1">
-      <c r="A135" s="1" t="s">
+      <c r="A132" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="136" spans="1:1" ht="15" customHeight="1">
-      <c r="A136" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" ht="15" customHeight="1">
-      <c r="A137" s="7" t="s">
-        <v>139</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -2148,7 +2124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9:E9"/>
     </sheetView>
   </sheetViews>
@@ -2165,13 +2141,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -2182,7 +2158,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>17</v>
@@ -2193,7 +2169,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>17</v>
@@ -2204,7 +2180,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>17</v>
@@ -2215,7 +2191,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>17</v>
@@ -2226,7 +2202,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>17</v>

</xml_diff>